<commit_message>
all functions are working till18th May 2025
</commit_message>
<xml_diff>
--- a/media/excel_templates/salary_template.xlsx
+++ b/media/excel_templates/salary_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1860" yWindow="1860" windowWidth="20460" windowHeight="10770" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="1" state="visible" r:id="rId1"/>
@@ -605,14 +605,14 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1076,7 +1076,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1093,10 +1093,10 @@
           <t>Employee ID</t>
         </is>
       </c>
-      <c r="B1" s="38" t="n"/>
+      <c r="B1" s="40" t="n"/>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>PCS0030</t>
+          <t>PCS0007</t>
         </is>
       </c>
       <c r="D1" s="51" t="inlineStr">
@@ -1119,7 +1119,7 @@
       <c r="B2" s="48" t="n"/>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Mr. Pravin Milake</t>
+          <t>Mr. Gaurab Pal</t>
         </is>
       </c>
       <c r="D2" s="50" t="n"/>
@@ -1134,7 +1134,7 @@
       <c r="B3" s="59" t="n"/>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>L2</t>
+          <t>L3</t>
         </is>
       </c>
       <c r="D3" s="45" t="n"/>
@@ -1149,10 +1149,10 @@
       <c r="B4" s="55" t="n"/>
       <c r="C4" s="56" t="n"/>
       <c r="D4" s="70" t="n">
-        <v>28200</v>
+        <v>41000</v>
       </c>
       <c r="E4" s="71" t="n">
-        <v>31802</v>
+        <v>46000</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1" thickBot="1">
@@ -1410,11 +1410,11 @@
         </is>
       </c>
       <c r="D17" s="72">
-        <f>(D7*12%)*12</f>
+        <f>D14*12</f>
         <v/>
       </c>
       <c r="E17" s="73">
-        <f>1800*12</f>
+        <f>E14*12</f>
         <v/>
       </c>
     </row>
@@ -1545,12 +1545,12 @@
           <t>Insurance</t>
         </is>
       </c>
-      <c r="C24" s="37" t="inlineStr">
+      <c r="C24" s="39" t="inlineStr">
         <is>
           <t>Insurance Benefits</t>
         </is>
       </c>
-      <c r="D24" s="38" t="n"/>
+      <c r="D24" s="40" t="n"/>
       <c r="E24" s="31" t="inlineStr">
         <is>
           <t>Amount</t>
@@ -1633,20 +1633,20 @@
           <t>Leaves</t>
         </is>
       </c>
-      <c r="C30" s="39" t="inlineStr">
+      <c r="C30" s="37" t="inlineStr">
         <is>
           <t>Leave (National monitised value of Earned Leaves for Full Years)</t>
         </is>
       </c>
-      <c r="D30" s="40" t="n"/>
+      <c r="D30" s="38" t="n"/>
       <c r="E30" s="83" t="n">
         <v>8000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C24:D24"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Added Expenses Approval flow
</commit_message>
<xml_diff>
--- a/media/excel_templates/salary_template.xlsx
+++ b/media/excel_templates/salary_template.xlsx
@@ -1096,7 +1096,7 @@
       <c r="B1" s="38" t="n"/>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>PCS0054</t>
+          <t>PCS0015</t>
         </is>
       </c>
       <c r="D1" s="51" t="inlineStr">
@@ -1119,7 +1119,7 @@
       <c r="B2" s="48" t="n"/>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Srushti Bagawe</t>
+          <t>Mr. Santhosh Saravanan</t>
         </is>
       </c>
       <c r="D2" s="50" t="n"/>
@@ -1149,10 +1149,10 @@
       <c r="B4" s="55" t="n"/>
       <c r="C4" s="56" t="n"/>
       <c r="D4" s="70" t="n">
-        <v>0</v>
+        <v>79200</v>
       </c>
       <c r="E4" s="71" t="n">
-        <v>0</v>
+        <v>99000</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1" thickBot="1">

</xml_diff>